<commit_message>
Reverted target release to 17, down from 21.
</commit_message>
<xml_diff>
--- a/TestExcel.xlsx
+++ b/TestExcel.xlsx
@@ -65,10 +65,10 @@
     <t>[[Singing, Walking, Programming]]</t>
   </si>
   <si>
-    <t>[[86.75, 90.45, 37.0]]</t>
-  </si>
-  <si>
-    <t>[{Maths,2010} ,{Comp Science,2012} ]</t>
+    <t>[[86.75, 37.0, 90.45]]</t>
+  </si>
+  <si>
+    <t>[{Comp Science : 2012} ,{Maths : 2010} ]</t>
   </si>
   <si>
     <t>Grace</t>
@@ -86,10 +86,10 @@
     <t>[[Working, Telling Stories, Relaxing]]</t>
   </si>
   <si>
-    <t>[[57.0, 70.0, 56.05]]</t>
-  </si>
-  <si>
-    <t>[{Abuse,2024} ,{Divorce,2023} ]</t>
+    <t>[[57.0, 56.05, 70.0]]</t>
+  </si>
+  <si>
+    <t>[{Divorce : 2023} ,{Abuse : 2024} ]</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added support for instance object as fields
</commit_message>
<xml_diff>
--- a/TestExcel.xlsx
+++ b/TestExcel.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+  <si>
+    <t>ID</t>
+  </si>
   <si>
     <t>NAME</t>
   </si>
@@ -47,6 +50,9 @@
     <t>COURSE</t>
   </si>
   <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
     <t>Manatsa</t>
   </si>
   <si>
@@ -65,10 +71,13 @@
     <t>[[Singing, Walking, Programming]]</t>
   </si>
   <si>
-    <t>[[86.75, 37.0, 90.45]]</t>
-  </si>
-  <si>
-    <t>[{Comp Science : 2012} ,{Maths : 2010} ]</t>
+    <t>[[86.75, 90.45, 37.0]]</t>
+  </si>
+  <si>
+    <t>[{Maths : 2010} ,{Comp Science : 2012} ]</t>
+  </si>
+  <si>
+    <t>[ { street : 735 Olive Street }  ,  { city : Sunway City }  ,  { country : Zimbabwe } ]</t>
   </si>
   <si>
     <t>Grace</t>
@@ -86,10 +95,10 @@
     <t>[[Working, Telling Stories, Relaxing]]</t>
   </si>
   <si>
-    <t>[[57.0, 56.05, 70.0]]</t>
-  </si>
-  <si>
-    <t>[{Divorce : 2023} ,{Abuse : 2024} ]</t>
+    <t>[[57.0, 70.0, 56.05]]</t>
+  </si>
+  <si>
+    <t>[{Abuse : 2024} ,{Divorce : 2023} ]</t>
   </si>
 </sst>
 </file>
@@ -134,7 +143,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -174,75 +183,89 @@
       <c r="K1" t="s" s="0">
         <v>10</v>
       </c>
+      <c r="L1" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s" s="0">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="B2" t="n" s="0">
+      <c r="A2" s="0"/>
+      <c r="B2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C2" t="n" s="0">
         <v>38.0</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="D2" t="b" s="0">
+      <c r="D2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E2" t="b" s="0">
         <v>1</v>
       </c>
-      <c r="E2" t="n" s="0">
+      <c r="F2" t="n" s="0">
         <v>1000.01</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>13</v>
-      </c>
       <c r="G2" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>21</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B3" t="n" s="0">
+      <c r="A3" s="0"/>
+      <c r="B3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C3" t="n" s="0">
         <v>30.0</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="D3" t="b" s="0">
+      <c r="D3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="E3" t="b" s="0">
         <v>1</v>
       </c>
-      <c r="E3" t="n" s="0">
+      <c r="F3" t="n" s="0">
         <v>620.14</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="G3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s" s="0">
         <v>21</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>